<commit_message>
ajout mcd, debut de code, et base de donnee mytown.sql
</commit_message>
<xml_diff>
--- a/Documents/src/Déscription des Use Case.xlsx
+++ b/Documents/src/Déscription des Use Case.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="14700" windowHeight="12240"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="14700" windowHeight="12240" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="8" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="143">
   <si>
     <t>Accès à l'agenda</t>
   </si>
@@ -430,6 +430,21 @@
   </si>
   <si>
     <t>Liste des Use Case Professionnel</t>
+  </si>
+  <si>
+    <t>id, nom</t>
+  </si>
+  <si>
+    <t>id, username, password</t>
+  </si>
+  <si>
+    <t>id, nom, type, adresse, date debut, date fin</t>
+  </si>
+  <si>
+    <t>id, nom, adresse, tel, lat, long, (lien carte)</t>
+  </si>
+  <si>
+    <t>id, nom, prenom, adresse, tel,categorie</t>
   </si>
 </sst>
 </file>
@@ -718,7 +733,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -729,43 +744,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -777,25 +783,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -806,9 +800,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -896,6 +887,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1286,277 +1298,285 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="71.5703125" style="57" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="57" customWidth="1"/>
-    <col min="4" max="4" width="1.7109375" style="49" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.7109375" style="49" customWidth="1"/>
-    <col min="7" max="7" width="21" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="49"/>
+    <col min="1" max="1" width="35.140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="71.5703125" style="49" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="49" customWidth="1"/>
+    <col min="4" max="4" width="1.7109375" style="41" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" style="41" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.7109375" style="41" customWidth="1"/>
+    <col min="7" max="7" width="21" style="41" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="41"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="55"/>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="56"/>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="56"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="56"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="37"/>
+      <c r="C8" s="57"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="60" t="s">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="C11" s="35"/>
+      <c r="C11" s="55" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="36"/>
+      <c r="C12" s="56"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="36"/>
+      <c r="C13" s="56"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="37"/>
+      <c r="C14" s="57"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="35"/>
+      <c r="C17" s="55" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C18" s="36"/>
+      <c r="C18" s="56"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="36"/>
+      <c r="C19" s="56"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C20" s="37"/>
+      <c r="C20" s="57"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="60" t="s">
+      <c r="A23" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="C23" s="35"/>
+      <c r="C23" s="55" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="56" t="s">
+      <c r="A24" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="C24" s="36"/>
+      <c r="C24" s="56"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="36"/>
+      <c r="C25" s="56"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="37"/>
+      <c r="C26" s="57"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="50" t="s">
+      <c r="C28" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="60" t="s">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="C29" s="35"/>
+      <c r="C29" s="55" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="36"/>
+      <c r="C30" s="56"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="36"/>
+      <c r="C31" s="56"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="37"/>
+      <c r="C32" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1575,183 +1595,183 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" style="49" customWidth="1"/>
-    <col min="2" max="2" width="71.5703125" style="49" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="49" customWidth="1"/>
-    <col min="4" max="4" width="1.7109375" style="49" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.7109375" style="49" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="49"/>
+    <col min="1" max="1" width="35.140625" style="41" customWidth="1"/>
+    <col min="2" max="2" width="71.5703125" style="41" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="41" customWidth="1"/>
+    <col min="4" max="4" width="1.7109375" style="41" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" style="41" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.7109375" style="41" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="41"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="53" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="42" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="27"/>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="28"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="28"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="37"/>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="42" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="35"/>
+      <c r="C10" s="27"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="36"/>
+      <c r="C11" s="28"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="C12" s="36"/>
+      <c r="C12" s="28"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="36"/>
+      <c r="C13" s="28"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="37"/>
+      <c r="C14" s="29"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="42" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="C17" s="35"/>
+      <c r="C17" s="27"/>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="36"/>
+      <c r="C18" s="28"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="36"/>
+      <c r="C19" s="28"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C20" s="37"/>
+      <c r="C20" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1766,103 +1786,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.5703125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.5703125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-    </row>
-    <row r="2" spans="1:3" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+    </row>
+    <row r="2" spans="1:3" s="41" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="26"/>
+      <c r="C4" s="58"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="26"/>
+      <c r="C5" s="58"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="59"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="59"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="23"/>
+      <c r="C8" s="60"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="61"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="11" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1871,483 +1891,485 @@
         <v>48</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
+      <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="26"/>
+      <c r="C13" s="58"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="8"/>
+      <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="8"/>
+      <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="26"/>
+      <c r="C24" s="58"/>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="8"/>
+      <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="12"/>
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="4"/>
+      <c r="C27" s="12"/>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="C28" s="12"/>
     </row>
     <row r="29" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="11"/>
+      <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:3" s="28" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14" t="s">
+    <row r="31" spans="1:3" s="21" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="38" t="s">
+    <row r="32" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="35"/>
-    </row>
-    <row r="33" spans="1:3" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="32" t="s">
+      <c r="C32" s="55"/>
+    </row>
+    <row r="33" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="36"/>
-    </row>
-    <row r="34" spans="1:3" s="28" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="32" t="s">
+      <c r="C33" s="56"/>
+    </row>
+    <row r="34" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="36"/>
-    </row>
-    <row r="35" spans="1:3" s="28" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="39" t="s">
+      <c r="C34" s="56"/>
+    </row>
+    <row r="35" spans="1:3" s="21" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="37"/>
-    </row>
-    <row r="36" spans="1:3" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="30"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="30"/>
-    </row>
-    <row r="37" spans="1:3" s="29" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="40" t="s">
+      <c r="C35" s="57"/>
+    </row>
+    <row r="36" spans="1:3" s="22" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="23"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+    </row>
+    <row r="37" spans="1:3" s="22" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="40" t="s">
+      <c r="C37" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="42" t="s">
+    <row r="38" spans="1:3" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="26"/>
-    </row>
-    <row r="39" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="44" t="s">
+      <c r="C38" s="58"/>
+    </row>
+    <row r="39" spans="1:3" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="4"/>
-    </row>
-    <row r="40" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="43" t="s">
+      <c r="C39" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="43" t="s">
+      <c r="C40" s="12"/>
+    </row>
+    <row r="41" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" spans="1:3" s="29" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="41" t="s">
+      <c r="C41" s="12"/>
+    </row>
+    <row r="42" spans="1:3" s="22" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="11"/>
-    </row>
-    <row r="43" spans="1:3" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="45"/>
-      <c r="B43" s="46"/>
-      <c r="C43" s="45"/>
+      <c r="C42" s="8"/>
+    </row>
+    <row r="43" spans="1:3" s="39" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="37"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
     </row>
     <row r="44" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="26"/>
+      <c r="C45" s="58"/>
     </row>
     <row r="46" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="4"/>
+      <c r="C46" s="12"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C47" s="4"/>
+      <c r="C47" s="12"/>
     </row>
     <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C48" s="4"/>
+      <c r="C48" s="12"/>
     </row>
     <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="4"/>
+      <c r="C49" s="12"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C50" s="8"/>
+      <c r="C50" s="3"/>
     </row>
     <row r="51" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="11"/>
+      <c r="C51" s="8"/>
     </row>
     <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C54" s="26"/>
+      <c r="C54" s="58"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C55" s="4"/>
+      <c r="C55" s="12"/>
     </row>
     <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C56" s="4"/>
+      <c r="C56" s="12"/>
     </row>
     <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C57" s="4"/>
+      <c r="C57" s="12"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C58" s="4"/>
+      <c r="C58" s="12"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C59" s="8"/>
+      <c r="C59" s="3"/>
     </row>
     <row r="60" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C60" s="11"/>
+      <c r="C60" s="8"/>
     </row>
     <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="25" t="s">
+      <c r="A63" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B63" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C63" s="26"/>
+      <c r="C63" s="58"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C64" s="4"/>
+      <c r="C64" s="12"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C65" s="4"/>
+      <c r="C65" s="12"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C66" s="4"/>
+      <c r="C66" s="12"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C67" s="4"/>
+      <c r="C67" s="12"/>
     </row>
     <row r="68" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="9" t="s">
+      <c r="A68" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="B68" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C68" s="11"/>
+      <c r="C68" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>